<commit_message>
convert Excel files for database seeding
</commit_message>
<xml_diff>
--- a/storage/app/keywords/1-2/231213 MSL vocabulary Geochemistry.xlsx
+++ b/storage/app/keywords/1-2/231213 MSL vocabulary Geochemistry.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/r_p_j_pijnenburg_uu_nl/Documents/EPOS-NL/07 Data/Metadata/231212 MSL vocabs 1.2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsh001\Projects\epos\storage\app\keywords\1-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="273" documentId="8_{FA7D9FDB-6B06-42E3-865F-9A1FB45F6CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DD2956A-29D6-4515-9D83-8EA0C99E7AD1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBF2352-5303-465F-B52E-145CFB213FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{F3BCA07C-F085-4C2E-91D1-BE33B4A72469}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21240" firstSheet="1" activeTab="2" xr2:uid="{F3BCA07C-F085-4C2E-91D1-BE33B4A72469}"/>
   </bookViews>
   <sheets>
     <sheet name="NB" sheetId="4" r:id="rId1"/>
-    <sheet name="Measurement technique" sheetId="3" r:id="rId2"/>
-    <sheet name="Measured property" sheetId="1" r:id="rId3"/>
+    <sheet name="Technique" sheetId="3" r:id="rId2"/>
+    <sheet name="Measured property #parameter" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -2101,10 +2101,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2459,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC320CFB-F604-4B25-9FB7-E194056F8F60}">
   <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -2988,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5493FE-C873-4AB4-80C7-643EAFBCE7F0}">
   <dimension ref="A1:D566"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A176" sqref="A176"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -5807,26 +5803,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="53df6a5f-9334-4503-a845-5e05459a4c71" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2184524c-f8db-481f-81f4-afb1a4d0a68c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED960ACB7111C64DB882066D7ADB6F8C" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="107e2b36e2bc44f1738303c28c94ab43">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2184524c-f8db-481f-81f4-afb1a4d0a68c" xmlns:ns3="53df6a5f-9334-4503-a845-5e05459a4c71" xmlns:ns4="6965ef5a-98c2-4976-9e1e-bc6458d0e33d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2d3d57358dacdc1002135371b44d032" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="2184524c-f8db-481f-81f4-afb1a4d0a68c"/>
@@ -6068,26 +6044,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19016B77-C79C-4CA2-BAD8-23965C5F48CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="53df6a5f-9334-4503-a845-5e05459a4c71"/>
-    <ds:schemaRef ds:uri="2184524c-f8db-481f-81f4-afb1a4d0a68c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="53df6a5f-9334-4503-a845-5e05459a4c71" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2184524c-f8db-481f-81f4-afb1a4d0a68c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8AFA186-28A2-4AC1-818D-45225B046A08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F3526C5-1E0A-49EF-80A7-38D4F70B5F7C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6105,4 +6082,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19016B77-C79C-4CA2-BAD8-23965C5F48CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="53df6a5f-9334-4503-a845-5e05459a4c71"/>
+    <ds:schemaRef ds:uri="2184524c-f8db-481f-81f4-afb1a4d0a68c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8AFA186-28A2-4AC1-818D-45225B046A08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>